<commit_message>
Error in hidden birth outcomes sheet of demo region 3
</commit_message>
<xml_diff>
--- a/inputs/demo_region3_input.xlsx
+++ b/inputs/demo_region3_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16C5D05-5D08-45AB-B390-A4DAEDB842BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75567921-2E5F-4DC3-B14A-031166FEA2C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" firstSheet="6" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="961" firstSheet="6" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <sheet name="Birth outcome risks" sheetId="66" state="hidden" r:id="rId20"/>
     <sheet name="Relative risks" sheetId="67" state="hidden" r:id="rId21"/>
     <sheet name="Odds ratios" sheetId="68" state="hidden" r:id="rId22"/>
-    <sheet name="Programs birth outcomes" sheetId="69" state="hidden" r:id="rId23"/>
+    <sheet name="Programs birth outcomes" sheetId="69" r:id="rId23"/>
     <sheet name="Programs anemia" sheetId="70" state="hidden" r:id="rId24"/>
     <sheet name="Programs wasting" sheetId="71" state="hidden" r:id="rId25"/>
     <sheet name="Programs for children" sheetId="72" r:id="rId26"/>
@@ -465,7 +465,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="270">
   <si>
     <t>year</t>
   </si>
@@ -1275,9 +1275,6 @@
   </si>
   <si>
     <t>Effectiveness incidence</t>
-  </si>
-  <si>
-    <t>A1</t>
   </si>
 </sst>
 </file>
@@ -11581,12 +11578,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11596,6 +11587,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -16315,8 +16312,8 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16359,8 +16356,8 @@
       <c r="D2" s="115">
         <v>0.21</v>
       </c>
-      <c r="E2" s="115" t="s">
-        <v>270</v>
+      <c r="E2" s="115">
+        <v>0</v>
       </c>
       <c r="F2" s="115">
         <v>0</v>
@@ -16564,8 +16561,8 @@
       <c r="C13" s="115">
         <v>1</v>
       </c>
-      <c r="D13" s="115" t="s">
-        <v>270</v>
+      <c r="D13" s="115">
+        <v>1</v>
       </c>
       <c r="E13" s="115">
         <v>1</v>
@@ -17491,7 +17488,7 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="111" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>